<commit_message>
Add new service types for UK INTRA
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK Intra.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/UK Intra.xlsx
@@ -599,9 +599,6 @@
     <t>FEDEX_NEXT_DAY_MID_MORNING, YOUR PACKAGING, Dry Ice</t>
   </si>
   <si>
-    <t>Friday Date</t>
-  </si>
-  <si>
     <t>Updated the EMEA and UK region test cases</t>
   </si>
   <si>
@@ -654,6 +651,9 @@
   </si>
   <si>
     <t>SaveLabel</t>
+  </si>
+  <si>
+    <t>Friday</t>
   </si>
 </sst>
 </file>
@@ -1612,7 +1612,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="26" applyFill="1" applyBorder="1"/>
@@ -1766,47 +1766,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="26" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="18" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="357" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1815,6 +1782,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="5" borderId="1" xfId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1839,24 +1812,54 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="26" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="17" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="17" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="18" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="26" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="357" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="383">
     <cellStyle name="Hyperlink 2" xfId="365"/>
@@ -2900,20 +2903,20 @@
     </row>
     <row r="9" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B9" s="61"/>
-      <c r="C9" s="98" t="s">
+      <c r="C9" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
-      <c r="G9" s="100" t="s">
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="H9" s="100"/>
-      <c r="I9" s="100"/>
-      <c r="J9" s="100"/>
-      <c r="K9" s="100"/>
-      <c r="L9" s="101"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="75"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -2941,20 +2944,20 @@
     </row>
     <row r="10" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
-      <c r="C10" s="85" t="s">
+      <c r="C10" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="87" t="s">
-        <v>194</v>
-      </c>
-      <c r="H10" s="87"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="87"/>
-      <c r="K10" s="87"/>
-      <c r="L10" s="88"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="78" t="s">
+        <v>193</v>
+      </c>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="79"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
@@ -2982,20 +2985,20 @@
     </row>
     <row r="11" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B11" s="61"/>
-      <c r="C11" s="85" t="s">
+      <c r="C11" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="87" t="s">
-        <v>193</v>
-      </c>
-      <c r="H11" s="87"/>
-      <c r="I11" s="87"/>
-      <c r="J11" s="87"/>
-      <c r="K11" s="87"/>
-      <c r="L11" s="88"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="78" t="s">
+        <v>192</v>
+      </c>
+      <c r="H11" s="78"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="79"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
@@ -3023,20 +3026,20 @@
     </row>
     <row r="12" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B12" s="61"/>
-      <c r="C12" s="85" t="s">
+      <c r="C12" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="87" t="s">
-        <v>192</v>
-      </c>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="88"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78" t="s">
+        <v>191</v>
+      </c>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="79"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
@@ -3064,20 +3067,20 @@
     </row>
     <row r="13" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B13" s="61"/>
-      <c r="C13" s="85" t="s">
+      <c r="C13" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="87" t="s">
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="87"/>
-      <c r="K13" s="87"/>
-      <c r="L13" s="88"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="79"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
@@ -3105,20 +3108,20 @@
     </row>
     <row r="14" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B14" s="61"/>
-      <c r="C14" s="85" t="s">
+      <c r="C14" s="76" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="89" t="s">
-        <v>206</v>
-      </c>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="90"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="82" t="s">
+        <v>205</v>
+      </c>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="83"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
@@ -3146,20 +3149,20 @@
     </row>
     <row r="15" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="61"/>
-      <c r="C15" s="91" t="s">
+      <c r="C15" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="92"/>
-      <c r="E15" s="92"/>
-      <c r="F15" s="92"/>
-      <c r="G15" s="93">
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="86">
         <v>42569</v>
       </c>
-      <c r="H15" s="94"/>
-      <c r="I15" s="94"/>
-      <c r="J15" s="94"/>
-      <c r="K15" s="94"/>
-      <c r="L15" s="95"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="88"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
@@ -3273,16 +3276,16 @@
       <c r="D18" s="49">
         <v>42135</v>
       </c>
-      <c r="E18" s="96" t="s">
-        <v>204</v>
-      </c>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="96"/>
-      <c r="J18" s="96"/>
-      <c r="K18" s="96"/>
-      <c r="L18" s="97"/>
+      <c r="E18" s="89" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
+      <c r="I18" s="89"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="89"/>
+      <c r="L18" s="90"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -3316,16 +3319,16 @@
       <c r="D19" s="9">
         <v>42047</v>
       </c>
-      <c r="E19" s="78" t="s">
+      <c r="E19" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="78"/>
-      <c r="I19" s="78"/>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="79"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="81"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
@@ -3359,16 +3362,16 @@
       <c r="D20" s="9">
         <v>42473</v>
       </c>
-      <c r="E20" s="78" t="s">
-        <v>191</v>
-      </c>
-      <c r="F20" s="78"/>
-      <c r="G20" s="78"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="79"/>
+      <c r="E20" s="80" t="s">
+        <v>190</v>
+      </c>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="80"/>
+      <c r="K20" s="80"/>
+      <c r="L20" s="81"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
@@ -3402,16 +3405,16 @@
       <c r="D21" s="9">
         <v>42500</v>
       </c>
-      <c r="E21" s="78" t="s">
-        <v>205</v>
-      </c>
-      <c r="F21" s="78"/>
-      <c r="G21" s="78"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="78"/>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
-      <c r="L21" s="79"/>
+      <c r="E21" s="80" t="s">
+        <v>204</v>
+      </c>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="80"/>
+      <c r="K21" s="80"/>
+      <c r="L21" s="81"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
@@ -3445,16 +3448,16 @@
       <c r="D22" s="48">
         <v>42569</v>
       </c>
-      <c r="E22" s="76" t="s">
-        <v>207</v>
-      </c>
-      <c r="F22" s="76"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="76"/>
-      <c r="K22" s="76"/>
-      <c r="L22" s="77"/>
+      <c r="E22" s="96" t="s">
+        <v>206</v>
+      </c>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="96"/>
+      <c r="J22" s="96"/>
+      <c r="K22" s="96"/>
+      <c r="L22" s="97"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
@@ -3484,14 +3487,14 @@
       <c r="B23" s="63"/>
       <c r="C23" s="66"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="78"/>
-      <c r="F23" s="78"/>
-      <c r="G23" s="78"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="78"/>
-      <c r="L23" s="79"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="80"/>
+      <c r="L23" s="81"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
@@ -3521,14 +3524,14 @@
       <c r="B24" s="63"/>
       <c r="C24" s="68"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="80"/>
-      <c r="I24" s="80"/>
-      <c r="J24" s="80"/>
-      <c r="K24" s="80"/>
-      <c r="L24" s="81"/>
+      <c r="E24" s="98"/>
+      <c r="F24" s="98"/>
+      <c r="G24" s="98"/>
+      <c r="H24" s="98"/>
+      <c r="I24" s="98"/>
+      <c r="J24" s="98"/>
+      <c r="K24" s="98"/>
+      <c r="L24" s="99"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -3558,14 +3561,14 @@
       <c r="B25" s="63"/>
       <c r="C25" s="68"/>
       <c r="D25" s="9"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="80"/>
-      <c r="H25" s="80"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="80"/>
-      <c r="K25" s="80"/>
-      <c r="L25" s="81"/>
+      <c r="E25" s="98"/>
+      <c r="F25" s="98"/>
+      <c r="G25" s="98"/>
+      <c r="H25" s="98"/>
+      <c r="I25" s="98"/>
+      <c r="J25" s="98"/>
+      <c r="K25" s="98"/>
+      <c r="L25" s="99"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
@@ -3595,14 +3598,14 @@
       <c r="B26" s="63"/>
       <c r="C26" s="69"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="82"/>
-      <c r="F26" s="82"/>
-      <c r="G26" s="82"/>
-      <c r="H26" s="82"/>
-      <c r="I26" s="82"/>
-      <c r="J26" s="82"/>
-      <c r="K26" s="82"/>
-      <c r="L26" s="83"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="100"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="101"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
@@ -3630,18 +3633,18 @@
     </row>
     <row r="27" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B27" s="61"/>
-      <c r="C27" s="84" t="s">
+      <c r="C27" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="71"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
-      <c r="G27" s="71"/>
-      <c r="H27" s="71"/>
-      <c r="I27" s="71"/>
-      <c r="J27" s="71"/>
-      <c r="K27" s="71"/>
-      <c r="L27" s="72"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="91"/>
+      <c r="G27" s="91"/>
+      <c r="H27" s="91"/>
+      <c r="I27" s="91"/>
+      <c r="J27" s="91"/>
+      <c r="K27" s="91"/>
+      <c r="L27" s="92"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
@@ -3669,18 +3672,18 @@
     </row>
     <row r="28" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B28" s="61"/>
-      <c r="C28" s="71" t="s">
+      <c r="C28" s="91" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="71"/>
-      <c r="L28" s="72"/>
+      <c r="D28" s="91"/>
+      <c r="E28" s="91"/>
+      <c r="F28" s="91"/>
+      <c r="G28" s="91"/>
+      <c r="H28" s="91"/>
+      <c r="I28" s="91"/>
+      <c r="J28" s="91"/>
+      <c r="K28" s="91"/>
+      <c r="L28" s="92"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
@@ -3708,18 +3711,18 @@
     </row>
     <row r="29" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="70"/>
-      <c r="C29" s="73" t="s">
+      <c r="C29" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="74"/>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="74"/>
-      <c r="K29" s="74"/>
-      <c r="L29" s="75"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="94"/>
+      <c r="I29" s="94"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="95"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
@@ -6453,12 +6456,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="G9:L9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:L10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G11:L11"/>
+    <mergeCell ref="C28:L28"/>
+    <mergeCell ref="C29:L29"/>
+    <mergeCell ref="E22:L22"/>
+    <mergeCell ref="E23:L23"/>
+    <mergeCell ref="E24:L24"/>
+    <mergeCell ref="E25:L25"/>
+    <mergeCell ref="E26:L26"/>
+    <mergeCell ref="C27:L27"/>
     <mergeCell ref="E21:L21"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="G12:L12"/>
@@ -6471,14 +6476,12 @@
     <mergeCell ref="E18:L18"/>
     <mergeCell ref="E19:L19"/>
     <mergeCell ref="E20:L20"/>
-    <mergeCell ref="C28:L28"/>
-    <mergeCell ref="C29:L29"/>
-    <mergeCell ref="E22:L22"/>
-    <mergeCell ref="E23:L23"/>
-    <mergeCell ref="E24:L24"/>
-    <mergeCell ref="E25:L25"/>
-    <mergeCell ref="E26:L26"/>
-    <mergeCell ref="C27:L27"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="G9:L9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:L10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:L11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6490,12 +6493,12 @@
   <dimension ref="A1:EL136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="105"/>
+    <col min="1" max="1" width="9.125" style="71"/>
     <col min="2" max="2" width="9.125" style="23" customWidth="1"/>
     <col min="3" max="3" width="51" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="57.375" style="23" customWidth="1"/>
@@ -6513,7 +6516,7 @@
   <sheetData>
     <row r="1" spans="1:129" s="15" customFormat="1" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
@@ -7167,7 +7170,7 @@
       <c r="A3" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="103" t="s">
         <v>132</v>
       </c>
       <c r="C3" s="36" t="s">
@@ -7206,14 +7209,14 @@
         <v>63</v>
       </c>
       <c r="P3" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q3" s="28" t="s">
         <v>137</v>
       </c>
       <c r="R3" s="34"/>
       <c r="S3" s="28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T3" s="34" t="s">
         <v>138</v>
@@ -7231,10 +7234,10 @@
         <v>63</v>
       </c>
       <c r="Y3" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z3" s="44" t="s">
         <v>197</v>
-      </c>
-      <c r="Z3" s="44" t="s">
-        <v>198</v>
       </c>
       <c r="AA3" s="34"/>
       <c r="AB3" s="34" t="s">
@@ -7433,14 +7436,14 @@
         <v>63</v>
       </c>
       <c r="P4" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q4" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R4" s="37"/>
       <c r="S4" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T4" s="37" t="s">
         <v>138</v>
@@ -7458,14 +7461,14 @@
         <v>63</v>
       </c>
       <c r="Y4" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z4" s="45" t="s">
         <v>199</v>
-      </c>
-      <c r="Z4" s="45" t="s">
-        <v>200</v>
       </c>
       <c r="AA4" s="37"/>
       <c r="AB4" s="37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AC4" s="37" t="s">
         <v>138</v>
@@ -7660,14 +7663,14 @@
         <v>63</v>
       </c>
       <c r="P5" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q5" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R5" s="37"/>
       <c r="S5" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T5" s="37" t="s">
         <v>138</v>
@@ -7685,10 +7688,10 @@
         <v>63</v>
       </c>
       <c r="Y5" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z5" s="45" t="s">
         <v>197</v>
-      </c>
-      <c r="Z5" s="45" t="s">
-        <v>198</v>
       </c>
       <c r="AA5" s="37"/>
       <c r="AB5" s="37" t="s">
@@ -7887,14 +7890,14 @@
         <v>63</v>
       </c>
       <c r="P6" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q6" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R6" s="37"/>
       <c r="S6" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T6" s="37" t="s">
         <v>138</v>
@@ -7912,14 +7915,14 @@
         <v>63</v>
       </c>
       <c r="Y6" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z6" s="45" t="s">
         <v>199</v>
-      </c>
-      <c r="Z6" s="45" t="s">
-        <v>200</v>
       </c>
       <c r="AA6" s="37"/>
       <c r="AB6" s="37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AC6" s="37" t="s">
         <v>138</v>
@@ -8114,14 +8117,14 @@
         <v>63</v>
       </c>
       <c r="P7" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q7" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R7" s="37"/>
       <c r="S7" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T7" s="37" t="s">
         <v>138</v>
@@ -8142,11 +8145,11 @@
         <v>149</v>
       </c>
       <c r="Z7" s="45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AA7" s="37"/>
       <c r="AB7" s="37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AC7" s="37" t="s">
         <v>138</v>
@@ -8341,14 +8344,14 @@
         <v>63</v>
       </c>
       <c r="P8" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q8" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R8" s="37"/>
       <c r="S8" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T8" s="37" t="s">
         <v>138</v>
@@ -8369,7 +8372,7 @@
         <v>157</v>
       </c>
       <c r="Z8" s="45" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AA8" s="37"/>
       <c r="AB8" s="37" t="s">
@@ -8568,14 +8571,14 @@
         <v>63</v>
       </c>
       <c r="P9" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q9" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R9" s="37"/>
       <c r="S9" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T9" s="37" t="s">
         <v>138</v>
@@ -8596,11 +8599,11 @@
         <v>149</v>
       </c>
       <c r="Z9" s="45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AA9" s="37"/>
       <c r="AB9" s="37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AC9" s="37" t="s">
         <v>138</v>
@@ -8793,14 +8796,14 @@
         <v>63</v>
       </c>
       <c r="P10" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q10" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R10" s="37"/>
       <c r="S10" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T10" s="37" t="s">
         <v>138</v>
@@ -8821,7 +8824,7 @@
         <v>157</v>
       </c>
       <c r="Z10" s="45" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AA10" s="37"/>
       <c r="AB10" s="37" t="s">
@@ -9018,14 +9021,14 @@
         <v>63</v>
       </c>
       <c r="P11" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q11" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R11" s="37"/>
       <c r="S11" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T11" s="37" t="s">
         <v>138</v>
@@ -9043,14 +9046,14 @@
         <v>63</v>
       </c>
       <c r="Y11" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z11" s="45" t="s">
         <v>199</v>
-      </c>
-      <c r="Z11" s="45" t="s">
-        <v>200</v>
       </c>
       <c r="AA11" s="37"/>
       <c r="AB11" s="37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AC11" s="37" t="s">
         <v>138</v>
@@ -9243,14 +9246,14 @@
         <v>63</v>
       </c>
       <c r="P12" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q12" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R12" s="37"/>
       <c r="S12" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T12" s="37" t="s">
         <v>138</v>
@@ -9474,14 +9477,14 @@
         <v>63</v>
       </c>
       <c r="P13" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q13" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R13" s="37"/>
       <c r="S13" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T13" s="37" t="s">
         <v>138</v>
@@ -9502,11 +9505,11 @@
         <v>149</v>
       </c>
       <c r="Z13" s="45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AA13" s="37"/>
       <c r="AB13" s="37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AC13" s="37" t="s">
         <v>138</v>
@@ -9705,14 +9708,14 @@
         <v>63</v>
       </c>
       <c r="P14" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q14" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R14" s="37"/>
       <c r="S14" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T14" s="37" t="s">
         <v>138</v>
@@ -9897,7 +9900,7 @@
       <c r="A15" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="B15" s="104"/>
+      <c r="B15" s="105"/>
       <c r="C15" s="36" t="s">
         <v>187</v>
       </c>
@@ -9909,7 +9912,7 @@
         <v>170</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="H15" s="37" t="s">
         <v>70</v>
@@ -9936,14 +9939,14 @@
         <v>63</v>
       </c>
       <c r="P15" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q15" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R15" s="37"/>
       <c r="S15" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T15" s="37" t="s">
         <v>138</v>
@@ -9961,14 +9964,14 @@
         <v>63</v>
       </c>
       <c r="Y15" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z15" s="45" t="s">
         <v>199</v>
-      </c>
-      <c r="Z15" s="45" t="s">
-        <v>200</v>
       </c>
       <c r="AA15" s="37"/>
       <c r="AB15" s="37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AC15" s="37" t="s">
         <v>138</v>
@@ -10128,7 +10131,7 @@
       <c r="A16" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="B16" s="104"/>
+      <c r="B16" s="105"/>
       <c r="C16" s="36" t="s">
         <v>188</v>
       </c>
@@ -10140,7 +10143,7 @@
         <v>171</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="H16" s="37" t="s">
         <v>70</v>
@@ -10167,14 +10170,14 @@
         <v>63</v>
       </c>
       <c r="P16" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q16" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R16" s="37"/>
       <c r="S16" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T16" s="37" t="s">
         <v>138</v>
@@ -10193,7 +10196,7 @@
         <v>157</v>
       </c>
       <c r="Z16" s="45" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AA16" s="37"/>
       <c r="AB16" s="37" t="s">
@@ -10349,7 +10352,7 @@
       <c r="A17" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="B17" s="104"/>
+      <c r="B17" s="105"/>
       <c r="C17" s="36" t="s">
         <v>189</v>
       </c>
@@ -10386,14 +10389,14 @@
         <v>63</v>
       </c>
       <c r="P17" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q17" s="29" t="s">
         <v>137</v>
       </c>
       <c r="R17" s="37"/>
       <c r="S17" s="29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T17" s="37" t="s">
         <v>138</v>
@@ -10580,7 +10583,7 @@
       <c r="A18" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="B18" s="103"/>
+      <c r="B18" s="106"/>
       <c r="C18" s="39" t="s">
         <v>187</v>
       </c>
@@ -10591,8 +10594,8 @@
       <c r="F18" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="G18" s="40" t="s">
-        <v>190</v>
+      <c r="G18" s="37" t="s">
+        <v>208</v>
       </c>
       <c r="H18" s="40" t="s">
         <v>70</v>
@@ -10619,14 +10622,14 @@
         <v>63</v>
       </c>
       <c r="P18" s="33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q18" s="30" t="s">
         <v>137</v>
       </c>
       <c r="R18" s="40"/>
       <c r="S18" s="30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T18" s="40" t="s">
         <v>138</v>
@@ -10645,11 +10648,11 @@
         <v>149</v>
       </c>
       <c r="Z18" s="46" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AA18" s="40"/>
       <c r="AB18" s="40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AC18" s="40" t="s">
         <v>138</v>

</xml_diff>